<commit_message>
data source ref forecast 2022
</commit_message>
<xml_diff>
--- a/reference/sales_report/BUDGET_TRANSPORT_2022.xlsx
+++ b/reference/sales_report/BUDGET_TRANSPORT_2022.xlsx
@@ -847,8 +847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>